<commit_message>
values and figs updated
</commit_message>
<xml_diff>
--- a/Documentation/Reports and Papers/Knee_Torque_Test/Tables/CoefficientTable.xlsx
+++ b/Documentation/Reports and Papers/Knee_Torque_Test/Tables/CoefficientTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Documentation\Reports and Papers\Knee_Torque_Test\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A9276F-9D31-41C9-9855-5A9AAB38F1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A63353-00C7-499D-A738-B69717ADF125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2286,7 +2286,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2473,12 +2473,24 @@
       <c r="D7" s="45">
         <v>41.5</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
+      <c r="E7" s="45">
+        <v>4.5197081384539599</v>
+      </c>
+      <c r="F7" s="45">
+        <v>3.9722004305122902</v>
+      </c>
+      <c r="G7" s="45">
+        <v>11.7412109674933</v>
+      </c>
+      <c r="H7" s="45">
+        <v>2.0417894891824799</v>
+      </c>
+      <c r="I7" s="45">
+        <v>0.84442496918497401</v>
+      </c>
+      <c r="J7" s="45">
+        <v>3.58761452437188</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="47"/>
@@ -2489,12 +2501,24 @@
       <c r="D8" s="45">
         <v>45.7</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
+      <c r="E8" s="45">
+        <v>1.99920194837266</v>
+      </c>
+      <c r="F8" s="45">
+        <v>0.89213700366721804</v>
+      </c>
+      <c r="G8" s="45">
+        <v>4.6092079774300299</v>
+      </c>
+      <c r="H8" s="45">
+        <v>0.89562322843932496</v>
+      </c>
+      <c r="I8" s="45">
+        <v>0.17904777063236799</v>
+      </c>
+      <c r="J8" s="45">
+        <v>1.8463910818920899</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="47"/>
@@ -2505,12 +2529,24 @@
       <c r="D9" s="45">
         <v>48</v>
       </c>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
+      <c r="E9" s="45">
+        <v>0.84470560285347895</v>
+      </c>
+      <c r="F9" s="45">
+        <v>0.23173900510265799</v>
+      </c>
+      <c r="G9" s="45">
+        <v>1.95145372442261</v>
+      </c>
+      <c r="H9" s="45">
+        <v>0.68178489628790195</v>
+      </c>
+      <c r="I9" s="45">
+        <v>0.150967387789747</v>
+      </c>
+      <c r="J9" s="45">
+        <v>2.0676835787835999</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="47"/>
@@ -2523,12 +2559,24 @@
       <c r="D10" s="45">
         <v>51.8</v>
       </c>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
+      <c r="E10" s="45">
+        <v>3.03222221811638</v>
+      </c>
+      <c r="F10" s="45">
+        <v>4.4855531007687901</v>
+      </c>
+      <c r="G10" s="45">
+        <v>5.5870357213666804</v>
+      </c>
+      <c r="H10" s="45">
+        <v>1.4609329694573101</v>
+      </c>
+      <c r="I10" s="45">
+        <v>1.0412488414276799</v>
+      </c>
+      <c r="J10" s="45">
+        <v>2.7551515923112402</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>